<commit_message>
Test Data is changed
</commit_message>
<xml_diff>
--- a/data/SuiteA.xlsx
+++ b/data/SuiteA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -571,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -891,7 +891,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>

</xml_diff>